<commit_message>
Cambiado al nuevo test.xlsc
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herminio/Git/citizens0/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
@@ -30,20 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>90500084Y</t>
-  </si>
-  <si>
-    <t>19160962F</t>
-  </si>
-  <si>
-    <t>09940449X</t>
-  </si>
-  <si>
     <t>C/ Federico García Lorca 2</t>
   </si>
   <si>
@@ -53,36 +39,15 @@
     <t>Av. De la Constitución 8</t>
   </si>
   <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
     <t>Juan</t>
   </si>
   <si>
-    <t>Torres Pardo</t>
-  </si>
-  <si>
     <t>Luis</t>
   </si>
   <si>
-    <t>López Fernando</t>
-  </si>
-  <si>
     <t>Ana</t>
   </si>
   <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
@@ -95,14 +60,38 @@
     <t>ana@example.com</t>
   </si>
   <si>
-    <t>Dirección postal</t>
+    <t>Localizacion</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>123a</t>
+  </si>
+  <si>
+    <t>77b</t>
+  </si>
+  <si>
+    <t>88c</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>2,ciudadano</t>
+  </si>
+  <si>
+    <t>3,sensor</t>
+  </si>
+  <si>
+    <t>1,entidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,11 +129,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -207,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,124 +407,101 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="1" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2">
-        <v>31330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25629</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3">
-        <v>21916</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>

</xml_diff>

<commit_message>
Cambios que se me pasaron hacer ayer
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando\git\Inci_e1a\Loader_e1a\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1215A172-192D-4091-A083-590567496CED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+  <calcPr calcId="125725"/>
+  <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Nombre</t>
   </si>
@@ -66,32 +72,65 @@
     <t>Identificador</t>
   </si>
   <si>
-    <t>123a</t>
-  </si>
-  <si>
-    <t>77b</t>
-  </si>
-  <si>
-    <t>88c</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
-    <t>2,ciudadano</t>
-  </si>
-  <si>
-    <t>3,sensor</t>
-  </si>
-  <si>
-    <t>1,entidad</t>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>usuarioLuis</t>
+  </si>
+  <si>
+    <t>sensorAna</t>
+  </si>
+  <si>
+    <t>juanSL</t>
+  </si>
+  <si>
+    <t>juan@uniovi.es</t>
+  </si>
+  <si>
+    <t>usuarioJuan</t>
+  </si>
+  <si>
+    <t>1.0,0.2</t>
+  </si>
+  <si>
+    <t>avisos@race.es</t>
+  </si>
+  <si>
+    <t>usuarioRace</t>
+  </si>
+  <si>
+    <t>1.123,-2.123</t>
+  </si>
+  <si>
+    <t>tecnico@copinsa.es</t>
+  </si>
+  <si>
+    <t>usuarioA6-PK27</t>
+  </si>
+  <si>
+    <t>23.231,123.2</t>
+  </si>
+  <si>
+    <t>RACE</t>
+  </si>
+  <si>
+    <t>SensorTemperatura-A6-PK27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +142,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,11 +176,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -407,28 +455,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,10 +491,10 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -456,13 +505,13 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -473,13 +522,13 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -490,18 +539,68 @@
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1"/>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C2" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>

</xml_diff>